<commit_message>
Work on CUDA and Posix
Completed work on CUDA Image processing and almost finished work on POSIX linear regression. Updated the time spreadsheets to include the new results.
</commit_message>
<xml_diff>
--- a/Image Times.xlsx
+++ b/Image Times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HPC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harpr\Desktop\HPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F102B8ED-722E-4FBF-8F9A-BC087F1554A2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{501D7A49-ED5E-4C17-8726-156F95DF4EBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27429" windowHeight="11323" xr2:uid="{82AAB230-F223-4C53-9302-D1B0E67C4653}"/>
   </bookViews>
@@ -49,6 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -145,6 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +466,16 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="5.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3828125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
@@ -497,7 +507,9 @@
       <c r="D2" s="6">
         <v>2.8823400000000001E-4</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2">
+        <v>7.9209999999999992E-6</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
@@ -512,7 +524,9 @@
       <c r="D3" s="6">
         <v>2.2912400000000001E-4</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3">
+        <v>7.5410000000000003E-6</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
@@ -527,7 +541,9 @@
       <c r="D4" s="6">
         <v>3.2516799999999997E-4</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3">
+        <v>9.6819999999999998E-6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
@@ -542,7 +558,9 @@
       <c r="D5" s="6">
         <v>2.1833599999999999E-4</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="3">
+        <v>8.9649999999999997E-6</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
@@ -557,7 +575,9 @@
       <c r="D6" s="6">
         <v>3.0080800000000001E-4</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3">
+        <v>8.8279999999999992E-6</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
@@ -572,7 +592,9 @@
       <c r="D7" s="6">
         <v>2.1165100000000001E-4</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3">
+        <v>8.5979999999999997E-6</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
@@ -587,7 +609,9 @@
       <c r="D8" s="6">
         <v>2.1242200000000001E-4</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3">
+        <v>1.0896999999999999E-5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
@@ -602,7 +626,9 @@
       <c r="D9" s="6">
         <v>1.4797000000000001E-4</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="3">
+        <v>6.5710000000000003E-6</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
@@ -617,7 +643,9 @@
       <c r="D10" s="6">
         <v>3.2101800000000001E-4</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3">
+        <v>1.0351E-5</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A11" s="3">
@@ -632,7 +660,9 @@
       <c r="D11" s="6">
         <v>3.1585899999999999E-4</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>7.8229999999999995E-6</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
@@ -650,12 +680,16 @@
         <f>AVERAGE(D2:D11)</f>
         <v>2.5705900000000002E-4</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="7">
+        <f>AVERAGE(E2:E11)</f>
+        <v>8.7176999999999979E-6</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update of CUDA Image
Time was not correctly worked out so program was modified to fix this issue. Journal and time document updated to include modifed code and updated results.
</commit_message>
<xml_diff>
--- a/Image Times.xlsx
+++ b/Image Times.xlsx
@@ -1,24 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harpr\Desktop\HPC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{501D7A49-ED5E-4C17-8726-156F95DF4EBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677597CB-BA13-4D3C-A999-74D15417DCB6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27429" windowHeight="11323" xr2:uid="{82AAB230-F223-4C53-9302-D1B0E67C4653}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -465,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86373DF4-FC05-47AC-85BC-F92253374999}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -508,7 +513,7 @@
         <v>2.8823400000000001E-4</v>
       </c>
       <c r="E2" s="2">
-        <v>7.9209999999999992E-6</v>
+        <v>1.53776E-4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -525,7 +530,7 @@
         <v>2.2912400000000001E-4</v>
       </c>
       <c r="E3" s="3">
-        <v>7.5410000000000003E-6</v>
+        <v>1.51986E-4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
@@ -542,7 +547,7 @@
         <v>3.2516799999999997E-4</v>
       </c>
       <c r="E4" s="3">
-        <v>9.6819999999999998E-6</v>
+        <v>1.4399000000000001E-4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
@@ -559,7 +564,7 @@
         <v>2.1833599999999999E-4</v>
       </c>
       <c r="E5" s="3">
-        <v>8.9649999999999997E-6</v>
+        <v>1.4198999999999999E-4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
@@ -576,7 +581,7 @@
         <v>3.0080800000000001E-4</v>
       </c>
       <c r="E6" s="3">
-        <v>8.8279999999999992E-6</v>
+        <v>1.46071E-4</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
@@ -593,7 +598,7 @@
         <v>2.1165100000000001E-4</v>
       </c>
       <c r="E7" s="3">
-        <v>8.5979999999999997E-6</v>
+        <v>1.4610799999999999E-4</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
@@ -610,7 +615,7 @@
         <v>2.1242200000000001E-4</v>
       </c>
       <c r="E8" s="3">
-        <v>1.0896999999999999E-5</v>
+        <v>1.43595E-4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
@@ -627,7 +632,7 @@
         <v>1.4797000000000001E-4</v>
       </c>
       <c r="E9" s="3">
-        <v>6.5710000000000003E-6</v>
+        <v>1.4576699999999999E-4</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.4">
@@ -644,7 +649,7 @@
         <v>3.2101800000000001E-4</v>
       </c>
       <c r="E10" s="3">
-        <v>1.0351E-5</v>
+        <v>1.4489E-4</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
@@ -661,7 +666,7 @@
         <v>3.1585899999999999E-4</v>
       </c>
       <c r="E11" s="3">
-        <v>7.8229999999999995E-6</v>
+        <v>1.5780699999999999E-4</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.45" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
@@ -682,7 +687,7 @@
       </c>
       <c r="E12" s="7">
         <f>AVERAGE(E2:E11)</f>
-        <v>8.7176999999999979E-6</v>
+        <v>1.4759800000000001E-4</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.4">

</xml_diff>